<commit_message>
code of 14th feb 2022
</commit_message>
<xml_diff>
--- a/RemoteMonitoringSystem/src/main/resources/rms_TestData/TestData.xlsx
+++ b/RemoteMonitoringSystem/src/main/resources/rms_TestData/TestData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="110">
   <si>
     <t>UserName</t>
   </si>
@@ -55,274 +55,214 @@
     <t>Total Devices</t>
   </si>
   <si>
+    <t>LoggedIn UserName</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>SiteName</t>
+  </si>
+  <si>
+    <t>AutomationTestSite</t>
+  </si>
+  <si>
+    <t>PanelName</t>
+  </si>
+  <si>
+    <t>AutomationTestPanel</t>
+  </si>
+  <si>
+    <t>DeviceName</t>
+  </si>
+  <si>
+    <t>AutomationTestDevice</t>
+  </si>
+  <si>
+    <t>MaxSlave</t>
+  </si>
+  <si>
+    <t>https</t>
+  </si>
+  <si>
+    <t>SIPL1000000005000001</t>
+  </si>
+  <si>
+    <t>Swetasdsf</t>
+  </si>
+  <si>
+    <t>Sjsipl45</t>
+  </si>
+  <si>
+    <t>test.txt</t>
+  </si>
+  <si>
+    <t>TimeZone</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Swrta</t>
+  </si>
+  <si>
+    <t>sweta</t>
+  </si>
+  <si>
+    <t>MQTTPort</t>
+  </si>
+  <si>
+    <t>Int_Timer</t>
+  </si>
+  <si>
+    <t>HTTP_URL</t>
+  </si>
+  <si>
+    <t>HTTP_Port</t>
+  </si>
+  <si>
+    <t>MQTT_KeyID</t>
+  </si>
+  <si>
+    <t>FTP_Username</t>
+  </si>
+  <si>
+    <t>FTP_Password</t>
+  </si>
+  <si>
+    <t>FTP_Filename</t>
+  </si>
+  <si>
+    <t>ClientName</t>
+  </si>
+  <si>
+    <t>Sweta</t>
+  </si>
+  <si>
+    <t>DashBoard_Name</t>
+  </si>
+  <si>
+    <t>DashBoard_Size</t>
+  </si>
+  <si>
+    <t>MeterName</t>
+  </si>
+  <si>
+    <t>MeterReading</t>
+  </si>
+  <si>
+    <t>Meter_Name</t>
+  </si>
+  <si>
+    <t>HPSIPL56</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>RTPL1000000006000001</t>
+  </si>
+  <si>
+    <t>SIPL1000000010000001</t>
+  </si>
+  <si>
+    <t>RTPL1000000002000001</t>
+  </si>
+  <si>
+    <t>METER902232</t>
+  </si>
+  <si>
+    <t>ELIP902992</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>11.11</t>
+  </si>
+  <si>
+    <t>AutoMeter1</t>
+  </si>
+  <si>
+    <t>Total Meters</t>
+  </si>
+  <si>
+    <t>Total DeviceTypes</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Testing Meter1</t>
+  </si>
+  <si>
+    <t>RP</t>
+  </si>
+  <si>
+    <t>Ravina Prajapati</t>
+  </si>
+  <si>
+    <t>MD Error Message</t>
+  </si>
+  <si>
+    <t>SlaveID</t>
+  </si>
+  <si>
+    <t>MaxRegister</t>
+  </si>
+  <si>
+    <t>RegisterColumns</t>
+  </si>
+  <si>
+    <t>RegName</t>
+  </si>
+  <si>
+    <t>AutoRegister1</t>
+  </si>
+  <si>
+    <t>RegNumber</t>
+  </si>
+  <si>
+    <t>Reg101</t>
+  </si>
+  <si>
+    <t>RegUnit</t>
+  </si>
+  <si>
+    <t>KG</t>
+  </si>
+  <si>
+    <t>RegThresold</t>
+  </si>
+  <si>
+    <t>LogoFile Columns</t>
+  </si>
+  <si>
+    <t>LogoFile Values</t>
+  </si>
+  <si>
     <t>Company Logo</t>
   </si>
   <si>
     <t>Total Site</t>
   </si>
   <si>
+    <t>Total Panel</t>
+  </si>
+  <si>
+    <t>Total Meter</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>Total Panel</t>
-  </si>
-  <si>
-    <t>Total Meter</t>
-  </si>
-  <si>
-    <t>LoggedIn UserName</t>
-  </si>
-  <si>
-    <t>Full Name</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Select Device Type.</t>
-  </si>
-  <si>
-    <t>Select Maximum Slave.</t>
-  </si>
-  <si>
-    <t>Select Baudrate.</t>
-  </si>
-  <si>
-    <t>Select Parity.</t>
-  </si>
-  <si>
-    <t>Interval Timer Required</t>
-  </si>
-  <si>
-    <t>Select APN</t>
-  </si>
-  <si>
-    <t>URL Is Required</t>
-  </si>
-  <si>
-    <t>Port Is Required</t>
-  </si>
-  <si>
-    <t>Key Id Is Required</t>
-  </si>
-  <si>
-    <t>Username Is Required</t>
-  </si>
-  <si>
-    <t>Password Is Required</t>
-  </si>
-  <si>
-    <t>CSVFileName Is Required</t>
-  </si>
-  <si>
-    <t>TimeZone Is Required.</t>
-  </si>
-  <si>
-    <t>DateTime Is Required.</t>
-  </si>
-  <si>
-    <t>Select Protocol.</t>
-  </si>
-  <si>
-    <t>Clientname Is Required.</t>
-  </si>
-  <si>
-    <t>Port Is Required.</t>
-  </si>
-  <si>
-    <t>Username Is Required.</t>
-  </si>
-  <si>
-    <t>Password Is Required.</t>
-  </si>
-  <si>
-    <t>SiteName</t>
-  </si>
-  <si>
-    <t>AutomationTestSite</t>
-  </si>
-  <si>
-    <t>PanelName</t>
-  </si>
-  <si>
-    <t>AutomationTestPanel</t>
-  </si>
-  <si>
-    <t>DeviceName</t>
-  </si>
-  <si>
-    <t>AutomationTestDevice</t>
-  </si>
-  <si>
-    <t>MaxSlave</t>
-  </si>
-  <si>
-    <t>https</t>
-  </si>
-  <si>
-    <t>SIPL1000000005000001</t>
-  </si>
-  <si>
-    <t>Swetasdsf</t>
-  </si>
-  <si>
-    <t>Sjsipl45</t>
-  </si>
-  <si>
-    <t>test.txt</t>
-  </si>
-  <si>
-    <t>TimeZone</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Swrta</t>
-  </si>
-  <si>
-    <t>sweta</t>
-  </si>
-  <si>
-    <t>MQTTPort</t>
-  </si>
-  <si>
-    <t>Int_Timer</t>
-  </si>
-  <si>
-    <t>HTTP_URL</t>
-  </si>
-  <si>
-    <t>HTTP_Port</t>
-  </si>
-  <si>
-    <t>MQTT_KeyID</t>
-  </si>
-  <si>
-    <t>FTP_Username</t>
-  </si>
-  <si>
-    <t>FTP_Password</t>
-  </si>
-  <si>
-    <t>FTP_Filename</t>
-  </si>
-  <si>
-    <t>ClientName</t>
-  </si>
-  <si>
-    <t>Sweta</t>
-  </si>
-  <si>
-    <t>DashBoard_Name</t>
-  </si>
-  <si>
-    <t>DashBoard_Size</t>
-  </si>
-  <si>
-    <t>MeterName</t>
-  </si>
-  <si>
-    <t>MeterReading</t>
-  </si>
-  <si>
-    <t>Meter_Name</t>
-  </si>
-  <si>
-    <t>HPSIPL56</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>RTPL1000000006000001</t>
-  </si>
-  <si>
-    <t>SIPL1000000010000001</t>
-  </si>
-  <si>
-    <t>RTPL1000000002000001</t>
-  </si>
-  <si>
-    <t>METER902232</t>
-  </si>
-  <si>
-    <t>ELIP902992</t>
-  </si>
-  <si>
-    <t>0.00</t>
-  </si>
-  <si>
-    <t>11.11</t>
-  </si>
-  <si>
-    <t>AutoMeter1</t>
-  </si>
-  <si>
-    <t>Total Meters</t>
-  </si>
-  <si>
-    <t>Total DeviceTypes</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Testing Meter1</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>RP</t>
-  </si>
-  <si>
-    <t>Ravina Prajapati</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>MD Error Message</t>
-  </si>
-  <si>
-    <t>SlaveID</t>
-  </si>
-  <si>
-    <t>MaxRegister</t>
-  </si>
-  <si>
-    <t>RegisterColumns</t>
-  </si>
-  <si>
-    <t>RegName</t>
-  </si>
-  <si>
-    <t>AutoRegister1</t>
-  </si>
-  <si>
-    <t>RegNumber</t>
-  </si>
-  <si>
-    <t>Reg101</t>
-  </si>
-  <si>
-    <t>RegUnit</t>
-  </si>
-  <si>
-    <t>KG</t>
-  </si>
-  <si>
-    <t>RegThresold</t>
+    <t>6</t>
   </si>
   <si>
     <t>File Name</t>
@@ -344,10 +284,70 @@
 Upload</t>
   </si>
   <si>
-    <t>LogoFile Columns</t>
-  </si>
-  <si>
-    <t>LogoFile Values</t>
+    <t>3</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Select Device Type.</t>
+  </si>
+  <si>
+    <t>Select Maximum Slave.</t>
+  </si>
+  <si>
+    <t>Select Baudrate.</t>
+  </si>
+  <si>
+    <t>Select Parity.</t>
+  </si>
+  <si>
+    <t>Interval Timer Required</t>
+  </si>
+  <si>
+    <t>Select APN</t>
+  </si>
+  <si>
+    <t>URL Is Required</t>
+  </si>
+  <si>
+    <t>Port Is Required</t>
+  </si>
+  <si>
+    <t>Key Id Is Required</t>
+  </si>
+  <si>
+    <t>Username Is Required</t>
+  </si>
+  <si>
+    <t>Password Is Required</t>
+  </si>
+  <si>
+    <t>CSVFileName Is Required</t>
+  </si>
+  <si>
+    <t>TimeZone Is Required.</t>
+  </si>
+  <si>
+    <t>DateTime Is Required.</t>
+  </si>
+  <si>
+    <t>Select Protocol.</t>
+  </si>
+  <si>
+    <t>Clientname Is Required.</t>
+  </si>
+  <si>
+    <t>Port Is Required.</t>
+  </si>
+  <si>
+    <t>Username Is Required.</t>
+  </si>
+  <si>
+    <t>Password Is Required.</t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
 </sst>
 </file>
@@ -671,7 +671,6 @@
     </xf>
     <xf applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="10" fillId="3" fontId="6" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -682,6 +681,7 @@
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="3" fontId="6" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="12" fillId="3" fontId="6" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Excel Built-in Normal 1" xfId="9"/>
@@ -1083,10 +1083,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row ht="16.5" r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1097,10 +1097,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1201,87 +1201,87 @@
   <sheetData>
     <row customFormat="1" ht="30" r="1" s="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="K1" s="16" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="L1" s="16" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="P1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="Q1" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="S1" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="T1" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="U1" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="V1" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="W1" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="R1" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="S1" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="T1" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="U1" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="V1" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="W1" s="26" t="s">
-        <v>99</v>
-      </c>
       <c r="X1" s="18" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
     </row>
     <row customFormat="1" ht="25.5" r="2" s="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="D2" s="17">
         <v>1000</v>
@@ -1290,43 +1290,43 @@
         <v>5</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="G2" s="17">
         <v>11</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="L2" s="17">
         <v>11</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="N2" s="17">
         <v>12</v>
       </c>
       <c r="O2" s="17" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="Q2" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="R2" s="25" t="s">
-        <v>85</v>
+        <v>54</v>
+      </c>
+      <c r="R2" s="24" t="s">
+        <v>58</v>
       </c>
       <c r="S2" s="17">
         <v>10</v>
@@ -1335,13 +1335,13 @@
         <v>10</v>
       </c>
       <c r="U2" s="17" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="V2" s="17" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="W2" s="17" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="X2" s="17">
         <v>5000</v>
@@ -1356,8 +1356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1380,318 +1380,186 @@
   </cols>
   <sheetData>
     <row customFormat="1" ht="15" r="1" s="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="26" t="s">
         <v>8</v>
       </c>
       <c r="I1" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row customFormat="1" r="2" s="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H2" t="s">
+        <v>104</v>
+      </c>
+      <c r="J2" t="s">
+        <v>109</v>
+      </c>
+      <c r="M2" t="s">
         <v>82</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="N2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row customFormat="1" r="3" s="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" t="s">
+        <v>105</v>
+      </c>
+      <c r="M3" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="L1" s="20" t="s">
+      <c r="N3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row customFormat="1" r="4" s="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H4" t="s">
+        <v>106</v>
+      </c>
+      <c r="M4" t="s">
+        <v>84</v>
+      </c>
+      <c r="N4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row customFormat="1" r="5" s="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row customFormat="1" r="6" s="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
         <v>94</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="H6" t="s">
         <v>108</v>
       </c>
-      <c r="N1" s="20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="14"/>
-      <c r="J2" t="s">
-        <v>90</v>
-      </c>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" t="s">
-        <v>102</v>
-      </c>
-      <c r="N2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" t="s">
-        <v>103</v>
-      </c>
-      <c r="N3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="14"/>
-      <c r="H4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="14"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" t="s">
-        <v>104</v>
-      </c>
-      <c r="N4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="14"/>
-      <c r="H5" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" s="14"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="14"/>
-      <c r="H6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="14"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
+    </row>
+    <row customFormat="1" r="7" s="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="14"/>
+        <v>95</v>
+      </c>
       <c r="H7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row customFormat="1" r="8" s="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row customFormat="1" r="9" s="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row customFormat="1" r="10" s="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F10" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row customFormat="1" r="11" s="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row customFormat="1" r="12" s="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row customFormat="1" r="13" s="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
+        <v>101</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.63541666666666663" footer="0" header="0" left="0" right="0" top="0.63541666666666663"/>
@@ -1723,36 +1591,36 @@
   <sheetData>
     <row ht="30" r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="F2" s="14"/>
     </row>
@@ -1760,48 +1628,48 @@
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" s="24"/>
+        <v>53</v>
+      </c>
+      <c r="E3" s="23"/>
       <c r="F3" s="14"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" s="24"/>
+        <v>52</v>
+      </c>
+      <c r="E4" s="23"/>
       <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E5" s="24"/>
+        <v>52</v>
+      </c>
+      <c r="E5" s="23"/>
       <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E6" s="24"/>
+        <v>52</v>
+      </c>
+      <c r="E6" s="23"/>
       <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1809,7 +1677,7 @@
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
-      <c r="E7" s="24"/>
+      <c r="E7" s="23"/>
       <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1817,7 +1685,7 @@
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="24"/>
+      <c r="E8" s="23"/>
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1825,7 +1693,7 @@
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
-      <c r="E9" s="24"/>
+      <c r="E9" s="23"/>
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1833,7 +1701,7 @@
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
-      <c r="E10" s="24"/>
+      <c r="E10" s="23"/>
       <c r="F10" s="14"/>
     </row>
   </sheetData>

</xml_diff>